<commit_message>
tidying things for report, changed to backward difference
</commit_message>
<xml_diff>
--- a/Week 2/Week2TransitionData.xlsx
+++ b/Week 2/Week2TransitionData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry\Desktop\Drive\Engineering - Part IIA\SA1 Wing Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Katja Ruda\Documents\3rd year\SA1\SA1-Group2-2023\Week 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AAB6B91-6B84-4762-B6D8-B733D1AA955F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B6D209-7956-4D51-AAF7-79BA52C37DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{81F25BA0-E1AF-4E3B-92B5-93553ACFC0AE}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{81F25BA0-E1AF-4E3B-92B5-93553ACFC0AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,10 +62,10 @@
     <t>Ex3</t>
   </si>
   <si>
-    <t>Transition occurs before separation at ReL &gt;= 3.3E5</t>
-  </si>
-  <si>
     <t>Ex5</t>
+  </si>
+  <si>
+    <t>Transition occurs before separation at ReL &gt;= 1.8E6</t>
   </si>
 </sst>
 </file>
@@ -421,16 +421,16 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="17.08984375" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,7 +447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1000000</v>
       </c>
@@ -461,7 +461,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1000000</v>
       </c>
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1000000</v>
       </c>
@@ -489,7 +489,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>10000000</v>
       </c>
@@ -503,7 +503,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>10000000</v>
       </c>
@@ -517,7 +517,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>10000000</v>
       </c>
@@ -531,7 +531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>100000000</v>
       </c>
@@ -545,7 +545,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>100000000</v>
       </c>
@@ -559,7 +559,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>100000000</v>
       </c>
@@ -573,7 +573,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -587,7 +587,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>100000</v>
       </c>
@@ -595,10 +595,10 @@
         <v>-0.5</v>
       </c>
       <c r="C13">
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>10000</v>
       </c>
@@ -606,10 +606,10 @@
         <v>-0.5</v>
       </c>
       <c r="C14">
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>1000</v>
       </c>
@@ -617,20 +617,20 @@
         <v>-0.5</v>
       </c>
       <c r="C15">
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>